<commit_message>
Changed MRI_SliceData to mm dimensions. Adjusted AnatomyScript to use MRI data. Currently getting weird flattened image.
</commit_message>
<xml_diff>
--- a/P&W MRI/MRI_SliceData.xlsx
+++ b/P&W MRI/MRI_SliceData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Fall 2017 Co-op\3DFrontalCortex\P&amp;W MRI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erica.nordin\Documents\3DFrontalCortex\P&amp;W MRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Figure</t>
   </si>
@@ -32,16 +32,19 @@
     <t>Bregma (mm, scaled)</t>
   </si>
   <si>
-    <t>Distance to next slice (mm, scaled)</t>
+    <t>Vertical size (mm)</t>
   </si>
   <si>
-    <t>Vertical shift from Figure 1 scale (cm, unscaled)</t>
+    <t>Horizontal size (mm)</t>
   </si>
   <si>
-    <t>Vertical size (cm, unscaled)</t>
+    <t>Vertical shift from Figure 1 scale (mm)</t>
   </si>
   <si>
-    <t>Horizontal size (cm, unscaled)</t>
+    <t>Bregma is taken directly off of the MRI images.</t>
+  </si>
+  <si>
+    <t>Other measurements are taken via Ctrl+E in Paint.</t>
   </si>
 </sst>
 </file>
@@ -393,22 +396,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" customWidth="1"/>
+    <col min="9" max="9" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,990 +420,1112 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>7.89</v>
       </c>
-      <c r="D2">
+      <c r="C2">
         <v>0</v>
       </c>
       <c r="F2">
-        <f>21.88*4</f>
-        <v>87.52</v>
+        <v>279.5</v>
       </c>
       <c r="G2">
-        <f xml:space="preserve"> 16.88*4</f>
-        <v>67.52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>215.9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>7.14</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>6.64</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>6.39</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>6.14</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>5.89</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>5.64</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>5.39</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>5.14</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>4.8899999999999997</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>4.6399999999999997</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>4.3899999999999997</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>4.1399999999999997</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>3.89</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>3.64</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>3.39</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>3.14</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>2.89</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>2.64</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>2.39</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <v>2.14</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <v>1.89</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>1.64</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <v>1.39</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <v>1.1399999999999999</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
         <v>0.89</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <v>0.64</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <v>0.39</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <v>-0.11</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32">
         <v>-0.36</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
         <v>-0.61</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
         <v>-0.86</v>
       </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
         <v>-1.1100000000000001</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
         <v>-1.36</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
         <v>-1.61</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
         <v>-1.86</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
         <v>-2.11</v>
       </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
         <v>-2.36</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
         <v>-2.61</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
         <v>-2.86</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
         <v>-3.11</v>
       </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
         <v>-3.36</v>
       </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
         <v>-3.61</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
         <v>-3.86</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
         <v>-4.1100000000000003</v>
       </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
         <v>-4.3600000000000003</v>
       </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
         <v>-4.6100000000000003</v>
       </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
         <v>-4.8600000000000003</v>
       </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
         <v>-5.1100000000000003</v>
       </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
         <v>-5.36</v>
       </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53">
         <v>-5.61</v>
       </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54">
         <v>-5.86</v>
       </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55">
         <v>-6.11</v>
       </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56">
         <v>-6.36</v>
       </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57">
         <v>-6.61</v>
       </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58">
         <v>-6.86</v>
       </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59">
         <v>-7.11</v>
       </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60">
         <v>-7.36</v>
       </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61">
         <v>-7.61</v>
       </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
         <v>-7.86</v>
       </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63">
         <v>-8.11</v>
       </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64">
         <v>-8.36</v>
       </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65">
         <v>-8.61</v>
       </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66">
         <v>-8.86</v>
       </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67">
         <v>-9.11</v>
       </c>
-      <c r="D67">
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <f>-180/10</f>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68">
         <v>-9.36</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <f t="shared" ref="C68:C97" si="0">-180/10</f>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69">
         <v>-9.61</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
         <v>-9.86</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71">
         <v>-10.11</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72">
         <v>-10.36</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73">
         <v>-10.61</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74">
         <v>-10.86</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75">
         <v>-11.11</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76">
         <v>-11.36</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77">
         <v>-11.61</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78">
         <v>-11.86</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79">
         <v>-12.11</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80">
         <v>-12.36</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81">
         <v>-12.61</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82">
         <v>-12.86</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83">
         <v>-13.11</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84">
         <v>-13.36</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85">
         <v>-13.61</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86">
         <v>-13.86</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87">
         <v>-14.11</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88">
         <v>-14.36</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89">
         <v>-14.61</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90">
         <v>-14.86</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91">
         <v>-15.11</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92">
         <v>-15.36</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93">
         <v>-15.61</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94">
         <v>-15.86</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95">
         <v>-16.11</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96">
         <v>-16.36</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97">
         <v>-16.61</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="0"/>
+        <v>-18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>